<commit_message>
Section 14 - Advanced Damage Techniques
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8fab4cc14023a0f/Documents/Unreal Projects/ManequimArena/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA8257CF-3422-44E9-8E6D-55A3A71C1BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{FA8257CF-3422-44E9-8E6D-55A3A71C1BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36D7032E-26BB-4107-871D-A06ABCE84EF9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43F676F-8328-43E6-B2DD-37F16397049A}"/>
+    <workbookView minimized="1" xWindow="-26355" yWindow="3105" windowWidth="12615" windowHeight="12420" xr2:uid="{D43F676F-8328-43E6-B2DD-37F16397049A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,10 +216,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -240,9 +240,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,7 +280,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -386,7 +386,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -528,7 +528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623F4491-A004-494A-88BD-60202D9FBB13}">
-  <dimension ref="A4:S63"/>
+  <dimension ref="A4:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +556,7 @@
     <col min="19" max="19" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -595,7 +595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -626,7 +626,7 @@
         <f>8+(D8/5)</f>
         <v>18</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="O5">
@@ -645,8 +645,12 @@
         <f>(O5*(P5+Q5)+R5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <f t="shared" ref="U5:U10" si="0">(100 - S5)/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -672,7 +676,7 @@
         <f>10+(C8/5)</f>
         <v>12</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="7"/>
       <c r="O6">
         <v>0.5</v>
       </c>
@@ -689,8 +693,12 @@
         <f>(O6*(P6+Q6)+R6)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -712,7 +720,7 @@
       <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="6"/>
+      <c r="N7" s="7"/>
       <c r="O7">
         <v>0.5</v>
       </c>
@@ -729,8 +737,12 @@
         <f>(O7*(P7+Q7)+R7)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
@@ -752,7 +764,7 @@
       <c r="I8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="6"/>
+      <c r="N8" s="7"/>
       <c r="O8">
         <v>0.5</v>
       </c>
@@ -769,8 +781,12 @@
         <f>(O8*(P8+Q8)+R8)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F9" s="4" t="s">
         <v>10</v>
       </c>
@@ -783,7 +799,7 @@
       <c r="I9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="6"/>
+      <c r="N9" s="7"/>
       <c r="O9">
         <v>0.5</v>
       </c>
@@ -800,8 +816,12 @@
         <f>(O9*(P9+Q9)+R9)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F10" s="4" t="s">
         <v>11</v>
       </c>
@@ -830,7 +850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
@@ -843,7 +863,7 @@
       <c r="I11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="O11">
@@ -862,8 +882,16 @@
         <f>(O11*(P11+Q11)+R11)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <f>(100 - S11)/100</f>
+        <v>0.95</v>
+      </c>
+      <c r="V11">
+        <f t="shared" ref="V11:V14" si="1">S11/100</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
@@ -876,7 +904,7 @@
       <c r="I12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="6"/>
+      <c r="N12" s="7"/>
       <c r="O12">
         <v>0.15</v>
       </c>
@@ -893,8 +921,16 @@
         <f>(O12*(P12+Q12)+R12)</f>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <f t="shared" ref="U12:U15" si="2">(100 - S12)/100</f>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="1"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
@@ -907,7 +943,7 @@
       <c r="I13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="6"/>
+      <c r="N13" s="7"/>
       <c r="O13">
         <v>0.15</v>
       </c>
@@ -924,8 +960,16 @@
         <f>(O13*(P13+Q13)+R13)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>0.92</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F14" s="4" t="s">
         <v>15</v>
       </c>
@@ -938,7 +982,7 @@
       <c r="I14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="6"/>
+      <c r="N14" s="7"/>
       <c r="O14">
         <v>0.15</v>
       </c>
@@ -955,9 +999,17 @@
         <f>(O14*(P14+Q14)+R14)</f>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N15" s="6"/>
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="1"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N15" s="7"/>
       <c r="O15">
         <v>0.15</v>
       </c>
@@ -974,8 +1026,16 @@
         <f>(O15*(P15+Q15)+R15)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>0.89</v>
+      </c>
+      <c r="V15">
+        <f>S15/100</f>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="O16" s="3" t="s">
         <v>21</v>
       </c>
@@ -993,7 +1053,7 @@
       </c>
     </row>
     <row r="17" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N17" s="7" t="s">
+      <c r="N17" s="6" t="s">
         <v>26</v>
       </c>
       <c r="O17">
@@ -1014,7 +1074,7 @@
       </c>
     </row>
     <row r="18" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N18" s="6"/>
+      <c r="N18" s="7"/>
       <c r="O18">
         <v>0.5</v>
       </c>
@@ -1033,7 +1093,7 @@
       </c>
     </row>
     <row r="19" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N19" s="6"/>
+      <c r="N19" s="7"/>
       <c r="O19">
         <v>0.5</v>
       </c>
@@ -1052,7 +1112,7 @@
       </c>
     </row>
     <row r="20" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N20" s="6"/>
+      <c r="N20" s="7"/>
       <c r="O20">
         <v>0.5</v>
       </c>
@@ -1071,7 +1131,7 @@
       </c>
     </row>
     <row r="21" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N21" s="6"/>
+      <c r="N21" s="7"/>
       <c r="O21">
         <v>0.5</v>
       </c>
@@ -1107,7 +1167,7 @@
       </c>
     </row>
     <row r="23" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N23" s="7" t="s">
+      <c r="N23" s="6" t="s">
         <v>27</v>
       </c>
       <c r="O23">
@@ -1128,7 +1188,7 @@
       </c>
     </row>
     <row r="24" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N24" s="6"/>
+      <c r="N24" s="7"/>
       <c r="O24">
         <v>1.4E-2</v>
       </c>
@@ -1147,7 +1207,7 @@
       </c>
     </row>
     <row r="25" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N25" s="6"/>
+      <c r="N25" s="7"/>
       <c r="O25">
         <v>1.4E-2</v>
       </c>
@@ -1166,7 +1226,7 @@
       </c>
     </row>
     <row r="26" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N26" s="6"/>
+      <c r="N26" s="7"/>
       <c r="O26">
         <v>1.4E-2</v>
       </c>
@@ -1185,7 +1245,7 @@
       </c>
     </row>
     <row r="27" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N27" s="6"/>
+      <c r="N27" s="7"/>
       <c r="O27">
         <v>1.4E-2</v>
       </c>
@@ -1221,7 +1281,7 @@
       </c>
     </row>
     <row r="29" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N29" s="7" t="s">
+      <c r="N29" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O29">
@@ -1242,7 +1302,7 @@
       </c>
     </row>
     <row r="30" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N30" s="6"/>
+      <c r="N30" s="7"/>
       <c r="O30">
         <v>0.1</v>
       </c>
@@ -1261,7 +1321,7 @@
       </c>
     </row>
     <row r="31" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N31" s="6"/>
+      <c r="N31" s="7"/>
       <c r="O31">
         <v>0.1</v>
       </c>
@@ -1280,7 +1340,7 @@
       </c>
     </row>
     <row r="32" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N32" s="6"/>
+      <c r="N32" s="7"/>
       <c r="O32">
         <v>0.1</v>
       </c>
@@ -1299,7 +1359,7 @@
       </c>
     </row>
     <row r="33" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N33" s="6"/>
+      <c r="N33" s="7"/>
       <c r="O33">
         <v>0.1</v>
       </c>
@@ -1335,7 +1395,7 @@
       </c>
     </row>
     <row r="35" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N35" s="7" t="s">
+      <c r="N35" s="6" t="s">
         <v>30</v>
       </c>
       <c r="O35">
@@ -1356,7 +1416,7 @@
       </c>
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N36" s="6"/>
+      <c r="N36" s="7"/>
       <c r="O36">
         <v>0.25</v>
       </c>
@@ -1375,7 +1435,7 @@
       </c>
     </row>
     <row r="37" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N37" s="6"/>
+      <c r="N37" s="7"/>
       <c r="O37">
         <v>0.25</v>
       </c>
@@ -1394,7 +1454,7 @@
       </c>
     </row>
     <row r="38" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N38" s="6"/>
+      <c r="N38" s="7"/>
       <c r="O38">
         <v>0.25</v>
       </c>
@@ -1413,7 +1473,7 @@
       </c>
     </row>
     <row r="39" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N39" s="6"/>
+      <c r="N39" s="7"/>
       <c r="O39">
         <v>0.25</v>
       </c>
@@ -1449,7 +1509,7 @@
       </c>
     </row>
     <row r="41" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N41" s="7" t="s">
+      <c r="N41" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O41">
@@ -1470,7 +1530,7 @@
       </c>
     </row>
     <row r="42" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N42" s="6"/>
+      <c r="N42" s="7"/>
       <c r="O42">
         <v>0.05</v>
       </c>
@@ -1489,7 +1549,7 @@
       </c>
     </row>
     <row r="43" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N43" s="6"/>
+      <c r="N43" s="7"/>
       <c r="O43">
         <v>0.05</v>
       </c>
@@ -1508,7 +1568,7 @@
       </c>
     </row>
     <row r="44" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N44" s="6"/>
+      <c r="N44" s="7"/>
       <c r="O44">
         <v>0.05</v>
       </c>
@@ -1527,7 +1587,7 @@
       </c>
     </row>
     <row r="45" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N45" s="6"/>
+      <c r="N45" s="7"/>
       <c r="O45">
         <v>0.05</v>
       </c>
@@ -1563,7 +1623,7 @@
       </c>
     </row>
     <row r="47" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N47" s="7" t="s">
+      <c r="N47" s="6" t="s">
         <v>32</v>
       </c>
       <c r="O47">
@@ -1584,7 +1644,7 @@
       </c>
     </row>
     <row r="48" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N48" s="6"/>
+      <c r="N48" s="7"/>
       <c r="O48">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1603,7 +1663,7 @@
       </c>
     </row>
     <row r="49" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N49" s="6"/>
+      <c r="N49" s="7"/>
       <c r="O49">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1622,7 +1682,7 @@
       </c>
     </row>
     <row r="50" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N50" s="6"/>
+      <c r="N50" s="7"/>
       <c r="O50">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1641,7 +1701,7 @@
       </c>
     </row>
     <row r="51" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N51" s="6"/>
+      <c r="N51" s="7"/>
       <c r="O51">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1677,7 +1737,7 @@
       </c>
     </row>
     <row r="53" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N53" s="7" t="s">
+      <c r="N53" s="6" t="s">
         <v>33</v>
       </c>
       <c r="O53">
@@ -1698,7 +1758,7 @@
       </c>
     </row>
     <row r="54" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N54" s="6"/>
+      <c r="N54" s="7"/>
       <c r="O54">
         <v>1.5</v>
       </c>
@@ -1717,7 +1777,7 @@
       </c>
     </row>
     <row r="55" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N55" s="6"/>
+      <c r="N55" s="7"/>
       <c r="O55">
         <v>1.5</v>
       </c>
@@ -1736,7 +1796,7 @@
       </c>
     </row>
     <row r="56" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N56" s="6"/>
+      <c r="N56" s="7"/>
       <c r="O56">
         <v>1.5</v>
       </c>
@@ -1755,7 +1815,7 @@
       </c>
     </row>
     <row r="57" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N57" s="6"/>
+      <c r="N57" s="7"/>
       <c r="O57">
         <v>1.5</v>
       </c>
@@ -1791,7 +1851,7 @@
       </c>
     </row>
     <row r="59" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N59" s="7" t="s">
+      <c r="N59" s="6" t="s">
         <v>34</v>
       </c>
       <c r="O59">
@@ -1812,7 +1872,7 @@
       </c>
     </row>
     <row r="60" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N60" s="6"/>
+      <c r="N60" s="7"/>
       <c r="O60">
         <v>1.5</v>
       </c>
@@ -1831,7 +1891,7 @@
       </c>
     </row>
     <row r="61" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N61" s="6"/>
+      <c r="N61" s="7"/>
       <c r="O61">
         <v>1.5</v>
       </c>
@@ -1850,7 +1910,7 @@
       </c>
     </row>
     <row r="62" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N62" s="6"/>
+      <c r="N62" s="7"/>
       <c r="O62">
         <v>1.5</v>
       </c>
@@ -1869,7 +1929,7 @@
       </c>
     </row>
     <row r="63" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N63" s="6"/>
+      <c r="N63" s="7"/>
       <c r="O63">
         <v>1.5</v>
       </c>

</xml_diff>